<commit_message>
Remove outdated documentation files and replace with updated content for event details. - Deleted tables.md and text_content.txt as they contained obsolete information. - Updated the Excel file with new event detail specifications. - Added new content.md file with comprehensive event details for initial display and button press events.
</commit_message>
<xml_diff>
--- a/sample/外部設計書_画面設計（あいうえお）.xlsx
+++ b/sample/外部設計書_画面設計（あいうえお）.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
   <si>
     <t xml:space="preserve">外部設計書</t>
   </si>
@@ -1097,10 +1097,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BE57"/>
+  <dimension ref="A1:BE63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AK47" activeCellId="0" sqref="AK47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1769,6 +1769,1140 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12"/>
+      <c r="E41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="16"/>
+      <c r="X41" s="16"/>
+      <c r="Y41" s="16"/>
+      <c r="Z41" s="16"/>
+      <c r="AA41" s="16"/>
+      <c r="AB41" s="16"/>
+      <c r="AC41" s="16"/>
+      <c r="AD41" s="16"/>
+      <c r="AE41" s="16"/>
+      <c r="AF41" s="16"/>
+      <c r="AG41" s="16"/>
+      <c r="AH41" s="16"/>
+      <c r="AI41" s="16"/>
+      <c r="AJ41" s="16"/>
+      <c r="AK41" s="16"/>
+      <c r="AL41" s="16"/>
+      <c r="AM41" s="16"/>
+      <c r="AN41" s="16"/>
+      <c r="AO41" s="16"/>
+      <c r="AP41" s="16"/>
+      <c r="AQ41" s="17"/>
+      <c r="BD41" s="14"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="12"/>
+      <c r="E42" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="18"/>
+      <c r="G42" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="19"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="19"/>
+      <c r="Y42" s="19"/>
+      <c r="Z42" s="19"/>
+      <c r="AA42" s="19"/>
+      <c r="AB42" s="19"/>
+      <c r="AC42" s="19"/>
+      <c r="AD42" s="19"/>
+      <c r="AE42" s="19"/>
+      <c r="AF42" s="19"/>
+      <c r="AG42" s="19"/>
+      <c r="AH42" s="19"/>
+      <c r="AI42" s="19"/>
+      <c r="AJ42" s="19"/>
+      <c r="AK42" s="19"/>
+      <c r="AL42" s="19"/>
+      <c r="AM42" s="19"/>
+      <c r="AN42" s="19"/>
+      <c r="AO42" s="19"/>
+      <c r="AP42" s="19"/>
+      <c r="AQ42" s="20"/>
+      <c r="BD42" s="14"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="12"/>
+      <c r="E43" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+      <c r="T43" s="19"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="19"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="19"/>
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AC43" s="19"/>
+      <c r="AD43" s="19"/>
+      <c r="AE43" s="19"/>
+      <c r="AF43" s="19"/>
+      <c r="AG43" s="19"/>
+      <c r="AH43" s="19"/>
+      <c r="AI43" s="19"/>
+      <c r="AJ43" s="19"/>
+      <c r="AK43" s="19"/>
+      <c r="AL43" s="19"/>
+      <c r="AM43" s="19"/>
+      <c r="AN43" s="19"/>
+      <c r="AO43" s="19"/>
+      <c r="AP43" s="19"/>
+      <c r="AQ43" s="20"/>
+      <c r="BD43" s="14"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="21"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="F44" s="23"/>
+      <c r="G44" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="24"/>
+      <c r="P44" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25"/>
+      <c r="S44" s="25"/>
+      <c r="T44" s="25"/>
+      <c r="U44" s="25"/>
+      <c r="V44" s="25"/>
+      <c r="W44" s="25"/>
+      <c r="X44" s="25"/>
+      <c r="Y44" s="25"/>
+      <c r="Z44" s="25"/>
+      <c r="AA44" s="25"/>
+      <c r="AB44" s="25"/>
+      <c r="AC44" s="25"/>
+      <c r="AD44" s="25"/>
+      <c r="AE44" s="25"/>
+      <c r="AF44" s="25"/>
+      <c r="AG44" s="25"/>
+      <c r="AH44" s="25"/>
+      <c r="AI44" s="25"/>
+      <c r="AJ44" s="25"/>
+      <c r="AK44" s="25"/>
+      <c r="AL44" s="25"/>
+      <c r="AM44" s="25"/>
+      <c r="AN44" s="25"/>
+      <c r="AO44" s="25"/>
+      <c r="AP44" s="25"/>
+      <c r="AQ44" s="26"/>
+      <c r="AR44" s="22"/>
+      <c r="AS44" s="22"/>
+      <c r="AT44" s="22"/>
+      <c r="AU44" s="22"/>
+      <c r="AV44" s="22"/>
+      <c r="AW44" s="22"/>
+      <c r="AX44" s="22"/>
+      <c r="AY44" s="22"/>
+      <c r="AZ44" s="22"/>
+      <c r="BA44" s="22"/>
+      <c r="BB44" s="22"/>
+      <c r="BC44" s="22"/>
+      <c r="BD44" s="27"/>
+      <c r="BE44" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="12"/>
+      <c r="E45" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="F45" s="18"/>
+      <c r="G45" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="19"/>
+      <c r="W45" s="19"/>
+      <c r="X45" s="19"/>
+      <c r="Y45" s="19"/>
+      <c r="Z45" s="19"/>
+      <c r="AA45" s="19"/>
+      <c r="AB45" s="19"/>
+      <c r="AC45" s="19"/>
+      <c r="AD45" s="19"/>
+      <c r="AE45" s="19"/>
+      <c r="AF45" s="19"/>
+      <c r="AG45" s="19"/>
+      <c r="AH45" s="19"/>
+      <c r="AI45" s="19"/>
+      <c r="AJ45" s="19"/>
+      <c r="AK45" s="19"/>
+      <c r="AL45" s="19"/>
+      <c r="AM45" s="19"/>
+      <c r="AN45" s="19"/>
+      <c r="AO45" s="19"/>
+      <c r="AP45" s="19"/>
+      <c r="AQ45" s="20"/>
+      <c r="BD45" s="14"/>
+      <c r="BE45" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="12"/>
+      <c r="BD46" s="14"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="12"/>
+      <c r="E47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD47" s="14"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="12"/>
+      <c r="BD48" s="14"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="12"/>
+      <c r="C49" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD49" s="14"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="12"/>
+      <c r="D50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD50" s="14"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="12"/>
+      <c r="BD51" s="14"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="12"/>
+      <c r="D52" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD52" s="14"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="12"/>
+      <c r="BD53" s="14"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="12"/>
+      <c r="E54" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BD54" s="14"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="12"/>
+      <c r="BD55" s="14"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="12"/>
+      <c r="E56" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BD56" s="14"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="12"/>
+      <c r="BD57" s="14"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="12"/>
+      <c r="D58" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="BD58" s="14"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="12"/>
+      <c r="BD59" s="14"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="12"/>
+      <c r="E60" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BD60" s="14"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="12"/>
+      <c r="BD61" s="14"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="12"/>
+      <c r="BD62" s="14"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="30"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="31"/>
+      <c r="K63" s="31"/>
+      <c r="L63" s="31"/>
+      <c r="M63" s="31"/>
+      <c r="N63" s="31"/>
+      <c r="O63" s="31"/>
+      <c r="P63" s="31"/>
+      <c r="Q63" s="31"/>
+      <c r="R63" s="31"/>
+      <c r="S63" s="31"/>
+      <c r="T63" s="31"/>
+      <c r="U63" s="31"/>
+      <c r="V63" s="31"/>
+      <c r="W63" s="31"/>
+      <c r="X63" s="31"/>
+      <c r="Y63" s="31"/>
+      <c r="Z63" s="31"/>
+      <c r="AA63" s="31"/>
+      <c r="AB63" s="31"/>
+      <c r="AC63" s="31"/>
+      <c r="AD63" s="31"/>
+      <c r="AE63" s="31"/>
+      <c r="AF63" s="31"/>
+      <c r="AG63" s="31"/>
+      <c r="AH63" s="31"/>
+      <c r="AI63" s="31"/>
+      <c r="AJ63" s="31"/>
+      <c r="AK63" s="31"/>
+      <c r="AL63" s="31"/>
+      <c r="AM63" s="31"/>
+      <c r="AN63" s="31"/>
+      <c r="AO63" s="31"/>
+      <c r="AP63" s="31"/>
+      <c r="AQ63" s="31"/>
+      <c r="AR63" s="31"/>
+      <c r="AS63" s="31"/>
+      <c r="AT63" s="31"/>
+      <c r="AU63" s="31"/>
+      <c r="AV63" s="31"/>
+      <c r="AW63" s="31"/>
+      <c r="AX63" s="31"/>
+      <c r="AY63" s="31"/>
+      <c r="AZ63" s="31"/>
+      <c r="BA63" s="31"/>
+      <c r="BB63" s="31"/>
+      <c r="BC63" s="31"/>
+      <c r="BD63" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="A2:AE2"/>
+    <mergeCell ref="AF2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AV2"/>
+    <mergeCell ref="A3:AE4"/>
+    <mergeCell ref="AF3:AL3"/>
+    <mergeCell ref="AM3:AP3"/>
+    <mergeCell ref="AQ3:AV3"/>
+    <mergeCell ref="AF4:AL4"/>
+    <mergeCell ref="AM4:AP4"/>
+    <mergeCell ref="AQ4:AV4"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:O17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:O18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:O19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:O20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:O21"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:O41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:O42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:O43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:O44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:O45"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:BE57"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="1" style="1" width="2.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="172" min="111" style="1" width="3.2"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="5" t="n">
+        <v>45292</v>
+      </c>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN3" s="6"/>
+      <c r="AO3" s="6"/>
+      <c r="AP3" s="6"/>
+      <c r="AQ3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="7"/>
+      <c r="AT3" s="7"/>
+      <c r="AU3" s="7"/>
+      <c r="AV3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="5" t="n">
+        <v>45413</v>
+      </c>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR4" s="7"/>
+      <c r="AS4" s="7"/>
+      <c r="AT4" s="7"/>
+      <c r="AU4" s="7"/>
+      <c r="AV4" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="10"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="10"/>
+      <c r="BB6" s="10"/>
+      <c r="BC6" s="10"/>
+      <c r="BD6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="BD7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12"/>
+      <c r="BD8" s="14"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12"/>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="BD9" s="14"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12"/>
+      <c r="BD10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12"/>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BD11" s="14"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12"/>
+      <c r="BD12" s="14"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12"/>
+      <c r="C13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD13" s="14"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12"/>
+      <c r="BD14" s="14"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12"/>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BD15" s="14"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12"/>
+      <c r="BD16" s="14"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12"/>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="16"/>
+      <c r="AC17" s="16"/>
+      <c r="AD17" s="16"/>
+      <c r="AE17" s="16"/>
+      <c r="AF17" s="16"/>
+      <c r="AG17" s="16"/>
+      <c r="AH17" s="16"/>
+      <c r="AI17" s="16"/>
+      <c r="AJ17" s="16"/>
+      <c r="AK17" s="16"/>
+      <c r="AL17" s="16"/>
+      <c r="AM17" s="16"/>
+      <c r="AN17" s="16"/>
+      <c r="AO17" s="16"/>
+      <c r="AP17" s="16"/>
+      <c r="AQ17" s="17"/>
+      <c r="BD17" s="14"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12"/>
+      <c r="E18" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="19"/>
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="19"/>
+      <c r="AG18" s="19"/>
+      <c r="AH18" s="19"/>
+      <c r="AI18" s="19"/>
+      <c r="AJ18" s="19"/>
+      <c r="AK18" s="19"/>
+      <c r="AL18" s="19"/>
+      <c r="AM18" s="19"/>
+      <c r="AN18" s="19"/>
+      <c r="AO18" s="19"/>
+      <c r="AP18" s="19"/>
+      <c r="AQ18" s="20"/>
+      <c r="BD18" s="14"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12"/>
+      <c r="E19" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19"/>
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="19"/>
+      <c r="AG19" s="19"/>
+      <c r="AH19" s="19"/>
+      <c r="AI19" s="19"/>
+      <c r="AJ19" s="19"/>
+      <c r="AK19" s="19"/>
+      <c r="AL19" s="19"/>
+      <c r="AM19" s="19"/>
+      <c r="AN19" s="19"/>
+      <c r="AO19" s="19"/>
+      <c r="AP19" s="19"/>
+      <c r="AQ19" s="20"/>
+      <c r="BD19" s="14"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="25"/>
+      <c r="AA20" s="25"/>
+      <c r="AB20" s="25"/>
+      <c r="AC20" s="25"/>
+      <c r="AD20" s="25"/>
+      <c r="AE20" s="25"/>
+      <c r="AF20" s="25"/>
+      <c r="AG20" s="25"/>
+      <c r="AH20" s="25"/>
+      <c r="AI20" s="25"/>
+      <c r="AJ20" s="25"/>
+      <c r="AK20" s="25"/>
+      <c r="AL20" s="25"/>
+      <c r="AM20" s="25"/>
+      <c r="AN20" s="25"/>
+      <c r="AO20" s="25"/>
+      <c r="AP20" s="25"/>
+      <c r="AQ20" s="26"/>
+      <c r="AR20" s="22"/>
+      <c r="AS20" s="22"/>
+      <c r="AT20" s="22"/>
+      <c r="AU20" s="22"/>
+      <c r="AV20" s="22"/>
+      <c r="AW20" s="22"/>
+      <c r="AX20" s="22"/>
+      <c r="AY20" s="22"/>
+      <c r="AZ20" s="22"/>
+      <c r="BA20" s="22"/>
+      <c r="BB20" s="22"/>
+      <c r="BC20" s="22"/>
+      <c r="BD20" s="27"/>
+      <c r="BE20" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12"/>
+      <c r="E21" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="19"/>
+      <c r="AC21" s="19"/>
+      <c r="AD21" s="19"/>
+      <c r="AE21" s="19"/>
+      <c r="AF21" s="19"/>
+      <c r="AG21" s="19"/>
+      <c r="AH21" s="19"/>
+      <c r="AI21" s="19"/>
+      <c r="AJ21" s="19"/>
+      <c r="AK21" s="19"/>
+      <c r="AL21" s="19"/>
+      <c r="AM21" s="19"/>
+      <c r="AN21" s="19"/>
+      <c r="AO21" s="19"/>
+      <c r="AP21" s="19"/>
+      <c r="AQ21" s="20"/>
+      <c r="BD21" s="14"/>
+      <c r="BE21" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12"/>
+      <c r="BD22" s="14"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12"/>
+      <c r="D23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BD23" s="14"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12"/>
+      <c r="BD24" s="14"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="12"/>
+      <c r="BD25" s="14"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="BD26" s="14"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12"/>
+      <c r="BD27" s="14"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="12"/>
+      <c r="C28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BD28" s="14"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="12"/>
+      <c r="BD29" s="14"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12"/>
+      <c r="C30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BD30" s="14"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12"/>
+      <c r="BD31" s="14"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="12"/>
+      <c r="B32" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="BD32" s="14"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="12"/>
+      <c r="BD33" s="14"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="12"/>
+      <c r="C34" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD34" s="14"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12"/>
+      <c r="D35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD35" s="14"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12"/>
+      <c r="BD36" s="14"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12"/>
+      <c r="D37" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="BD37" s="14"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="12"/>
+      <c r="BD38" s="14"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="12"/>
+      <c r="E39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD39" s="14"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="12"/>
+      <c r="BD40" s="14"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="12"/>
       <c r="E41" s="1" t="s">
         <v>36</v>
       </c>
@@ -1799,7 +2933,7 @@
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12"/>
       <c r="D46" s="29" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="BD46" s="14"/>
     </row>
@@ -1810,7 +2944,7 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12"/>
       <c r="E48" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="BD48" s="14"/>
     </row>
@@ -1939,861 +3073,6 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:BE57"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="1" style="1" width="2.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="172" min="111" style="1" width="3.2"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2"/>
-      <c r="AT2" s="2"/>
-      <c r="AU2" s="2"/>
-      <c r="AV2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="5" t="n">
-        <v>45292</v>
-      </c>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5"/>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="5"/>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5"/>
-      <c r="AM3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="6"/>
-      <c r="AP3" s="6"/>
-      <c r="AQ3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="AR3" s="7"/>
-      <c r="AS3" s="7"/>
-      <c r="AT3" s="7"/>
-      <c r="AU3" s="7"/>
-      <c r="AV3" s="7"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="5" t="n">
-        <v>45413</v>
-      </c>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="5"/>
-      <c r="AI4" s="5"/>
-      <c r="AJ4" s="5"/>
-      <c r="AK4" s="5"/>
-      <c r="AL4" s="5"/>
-      <c r="AM4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="AN4" s="8"/>
-      <c r="AO4" s="8"/>
-      <c r="AP4" s="8"/>
-      <c r="AQ4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="7"/>
-      <c r="AU4" s="7"/>
-      <c r="AV4" s="7"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="10"/>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="10"/>
-      <c r="AG6" s="10"/>
-      <c r="AH6" s="10"/>
-      <c r="AI6" s="10"/>
-      <c r="AJ6" s="10"/>
-      <c r="AK6" s="10"/>
-      <c r="AL6" s="10"/>
-      <c r="AM6" s="10"/>
-      <c r="AN6" s="10"/>
-      <c r="AO6" s="10"/>
-      <c r="AP6" s="10"/>
-      <c r="AQ6" s="10"/>
-      <c r="AR6" s="10"/>
-      <c r="AS6" s="10"/>
-      <c r="AT6" s="10"/>
-      <c r="AU6" s="10"/>
-      <c r="AV6" s="10"/>
-      <c r="AW6" s="10"/>
-      <c r="AX6" s="10"/>
-      <c r="AY6" s="10"/>
-      <c r="AZ6" s="10"/>
-      <c r="BA6" s="10"/>
-      <c r="BB6" s="10"/>
-      <c r="BC6" s="10"/>
-      <c r="BD6" s="11"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="BD7" s="14"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
-      <c r="BD8" s="14"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
-      <c r="C9" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="BD9" s="14"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
-      <c r="BD10" s="14"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="D11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="BD11" s="14"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="BD12" s="14"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="C13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="BD13" s="14"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
-      <c r="BD14" s="14"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="D15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BD15" s="14"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
-      <c r="BD16" s="14"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
-      <c r="E17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="16"/>
-      <c r="Y17" s="16"/>
-      <c r="Z17" s="16"/>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="16"/>
-      <c r="AC17" s="16"/>
-      <c r="AD17" s="16"/>
-      <c r="AE17" s="16"/>
-      <c r="AF17" s="16"/>
-      <c r="AG17" s="16"/>
-      <c r="AH17" s="16"/>
-      <c r="AI17" s="16"/>
-      <c r="AJ17" s="16"/>
-      <c r="AK17" s="16"/>
-      <c r="AL17" s="16"/>
-      <c r="AM17" s="16"/>
-      <c r="AN17" s="16"/>
-      <c r="AO17" s="16"/>
-      <c r="AP17" s="16"/>
-      <c r="AQ17" s="17"/>
-      <c r="BD17" s="14"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
-      <c r="E18" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
-      <c r="W18" s="19"/>
-      <c r="X18" s="19"/>
-      <c r="Y18" s="19"/>
-      <c r="Z18" s="19"/>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="19"/>
-      <c r="AC18" s="19"/>
-      <c r="AD18" s="19"/>
-      <c r="AE18" s="19"/>
-      <c r="AF18" s="19"/>
-      <c r="AG18" s="19"/>
-      <c r="AH18" s="19"/>
-      <c r="AI18" s="19"/>
-      <c r="AJ18" s="19"/>
-      <c r="AK18" s="19"/>
-      <c r="AL18" s="19"/>
-      <c r="AM18" s="19"/>
-      <c r="AN18" s="19"/>
-      <c r="AO18" s="19"/>
-      <c r="AP18" s="19"/>
-      <c r="AQ18" s="20"/>
-      <c r="BD18" s="14"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
-      <c r="E19" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="X19" s="19"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="19"/>
-      <c r="AA19" s="19"/>
-      <c r="AB19" s="19"/>
-      <c r="AC19" s="19"/>
-      <c r="AD19" s="19"/>
-      <c r="AE19" s="19"/>
-      <c r="AF19" s="19"/>
-      <c r="AG19" s="19"/>
-      <c r="AH19" s="19"/>
-      <c r="AI19" s="19"/>
-      <c r="AJ19" s="19"/>
-      <c r="AK19" s="19"/>
-      <c r="AL19" s="19"/>
-      <c r="AM19" s="19"/>
-      <c r="AN19" s="19"/>
-      <c r="AO19" s="19"/>
-      <c r="AP19" s="19"/>
-      <c r="AQ19" s="20"/>
-      <c r="BD19" s="14"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="25"/>
-      <c r="U20" s="25"/>
-      <c r="V20" s="25"/>
-      <c r="W20" s="25"/>
-      <c r="X20" s="25"/>
-      <c r="Y20" s="25"/>
-      <c r="Z20" s="25"/>
-      <c r="AA20" s="25"/>
-      <c r="AB20" s="25"/>
-      <c r="AC20" s="25"/>
-      <c r="AD20" s="25"/>
-      <c r="AE20" s="25"/>
-      <c r="AF20" s="25"/>
-      <c r="AG20" s="25"/>
-      <c r="AH20" s="25"/>
-      <c r="AI20" s="25"/>
-      <c r="AJ20" s="25"/>
-      <c r="AK20" s="25"/>
-      <c r="AL20" s="25"/>
-      <c r="AM20" s="25"/>
-      <c r="AN20" s="25"/>
-      <c r="AO20" s="25"/>
-      <c r="AP20" s="25"/>
-      <c r="AQ20" s="26"/>
-      <c r="AR20" s="22"/>
-      <c r="AS20" s="22"/>
-      <c r="AT20" s="22"/>
-      <c r="AU20" s="22"/>
-      <c r="AV20" s="22"/>
-      <c r="AW20" s="22"/>
-      <c r="AX20" s="22"/>
-      <c r="AY20" s="22"/>
-      <c r="AZ20" s="22"/>
-      <c r="BA20" s="22"/>
-      <c r="BB20" s="22"/>
-      <c r="BC20" s="22"/>
-      <c r="BD20" s="27"/>
-      <c r="BE20" s="28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
-      <c r="E21" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="19"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="19"/>
-      <c r="AD21" s="19"/>
-      <c r="AE21" s="19"/>
-      <c r="AF21" s="19"/>
-      <c r="AG21" s="19"/>
-      <c r="AH21" s="19"/>
-      <c r="AI21" s="19"/>
-      <c r="AJ21" s="19"/>
-      <c r="AK21" s="19"/>
-      <c r="AL21" s="19"/>
-      <c r="AM21" s="19"/>
-      <c r="AN21" s="19"/>
-      <c r="AO21" s="19"/>
-      <c r="AP21" s="19"/>
-      <c r="AQ21" s="20"/>
-      <c r="BD21" s="14"/>
-      <c r="BE21" s="28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
-      <c r="BD22" s="14"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
-      <c r="D23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BD23" s="14"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12"/>
-      <c r="BD24" s="14"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12"/>
-      <c r="BD25" s="14"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="BD26" s="14"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
-      <c r="BD27" s="14"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12"/>
-      <c r="C28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="BD28" s="14"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12"/>
-      <c r="BD29" s="14"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12"/>
-      <c r="C30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="BD30" s="14"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12"/>
-      <c r="BD31" s="14"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="BD32" s="14"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
-      <c r="BD33" s="14"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
-      <c r="C34" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="BD34" s="14"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
-      <c r="D35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD35" s="14"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
-      <c r="BD36" s="14"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
-      <c r="D37" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="BD37" s="14"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
-      <c r="BD38" s="14"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12"/>
-      <c r="E39" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="BD39" s="14"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12"/>
-      <c r="BD40" s="14"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
-      <c r="E41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD41" s="14"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
-      <c r="BD42" s="14"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12"/>
-      <c r="C43" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BD43" s="14"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12"/>
-      <c r="D44" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD44" s="14"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="12"/>
-      <c r="BD45" s="14"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="12"/>
-      <c r="D46" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="BD46" s="14"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12"/>
-      <c r="BD47" s="14"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="12"/>
-      <c r="E48" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BD48" s="14"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="12"/>
-      <c r="BD49" s="14"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="12"/>
-      <c r="E50" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD50" s="14"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="12"/>
-      <c r="BD51" s="14"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="12"/>
-      <c r="D52" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="BD52" s="14"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="12"/>
-      <c r="BD53" s="14"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="12"/>
-      <c r="E54" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD54" s="14"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="12"/>
-      <c r="BD55" s="14"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="12"/>
-      <c r="BD56" s="14"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="30"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
-      <c r="J57" s="31"/>
-      <c r="K57" s="31"/>
-      <c r="L57" s="31"/>
-      <c r="M57" s="31"/>
-      <c r="N57" s="31"/>
-      <c r="O57" s="31"/>
-      <c r="P57" s="31"/>
-      <c r="Q57" s="31"/>
-      <c r="R57" s="31"/>
-      <c r="S57" s="31"/>
-      <c r="T57" s="31"/>
-      <c r="U57" s="31"/>
-      <c r="V57" s="31"/>
-      <c r="W57" s="31"/>
-      <c r="X57" s="31"/>
-      <c r="Y57" s="31"/>
-      <c r="Z57" s="31"/>
-      <c r="AA57" s="31"/>
-      <c r="AB57" s="31"/>
-      <c r="AC57" s="31"/>
-      <c r="AD57" s="31"/>
-      <c r="AE57" s="31"/>
-      <c r="AF57" s="31"/>
-      <c r="AG57" s="31"/>
-      <c r="AH57" s="31"/>
-      <c r="AI57" s="31"/>
-      <c r="AJ57" s="31"/>
-      <c r="AK57" s="31"/>
-      <c r="AL57" s="31"/>
-      <c r="AM57" s="31"/>
-      <c r="AN57" s="31"/>
-      <c r="AO57" s="31"/>
-      <c r="AP57" s="31"/>
-      <c r="AQ57" s="31"/>
-      <c r="AR57" s="31"/>
-      <c r="AS57" s="31"/>
-      <c r="AT57" s="31"/>
-      <c r="AU57" s="31"/>
-      <c r="AV57" s="31"/>
-      <c r="AW57" s="31"/>
-      <c r="AX57" s="31"/>
-      <c r="AY57" s="31"/>
-      <c r="AZ57" s="31"/>
-      <c r="BA57" s="31"/>
-      <c r="BB57" s="31"/>
-      <c r="BC57" s="31"/>
-      <c r="BD57" s="32"/>
-    </row>
-  </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A2:AE2"/>
-    <mergeCell ref="AF2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="A3:AE4"/>
-    <mergeCell ref="AF3:AL3"/>
-    <mergeCell ref="AM3:AP3"/>
-    <mergeCell ref="AQ3:AV3"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AM4:AP4"/>
-    <mergeCell ref="AQ4:AV4"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:O17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:O18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:O19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:O20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:O21"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>

</xml_diff>